<commit_message>
fixed the database issue
</commit_message>
<xml_diff>
--- a/openmrs/src/main/resources/testData/PASS_OpenMRS.xlsx
+++ b/openmrs/src/main/resources/testData/PASS_OpenMRS.xlsx
@@ -4,55 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="registerNewPatient" sheetId="1" r:id="rId1"/>
-    <sheet name="testData" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="newCustomer" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>Check1</t>
-  </si>
-  <si>
-    <t>Check2</t>
-  </si>
-  <si>
-    <t>Check3</t>
-  </si>
-  <si>
-    <t>OK1</t>
-  </si>
-  <si>
-    <t>OK2</t>
-  </si>
-  <si>
-    <t>OK3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Gender</t>
   </si>
@@ -84,22 +47,43 @@
     <t>Password</t>
   </si>
   <si>
-    <t>NoteBook</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
-    <t>NoteBook, Address</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
-    <t>notebook@test.com</t>
-  </si>
-  <si>
     <t>notebook</t>
+  </si>
+  <si>
+    <t>NoteBook Address</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>12/31/2020</t>
+  </si>
+  <si>
+    <t>NoteBookApp</t>
+  </si>
+  <si>
+    <t>NoteBookA</t>
+  </si>
+  <si>
+    <t>NoteBookAp</t>
+  </si>
+  <si>
+    <t>notebookAeqe@test.com</t>
+  </si>
+  <si>
+    <t>notebookAeqg@test.com</t>
+  </si>
+  <si>
+    <t>notebookAeqd@test.com</t>
   </si>
 </sst>
 </file>
@@ -150,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,8 +142,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,69 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,77 +464,143 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44196</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2">
-        <v>12345</v>
-      </c>
-      <c r="H2">
-        <v>1234</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>